<commit_message>
cleaned the code a bit
</commit_message>
<xml_diff>
--- a/data_processing/Sampledata_Comet_Allcolumns_updated28thAug.xlsx
+++ b/data_processing/Sampledata_Comet_Allcolumns_updated28thAug.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\azfarjef\42KL\DHL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\azfarjef\42KL\DHL\data_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A483ADF8-B587-4F8B-8FF6-4C94C9177D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A448F63-E8DA-4FC4-848C-91568A3DC45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30023" yWindow="-367" windowWidth="8680" windowHeight="13925" firstSheet="1" activeTab="5" xr2:uid="{42CE140A-3AB5-438F-8412-76FAA93178C8}"/>
+    <workbookView xWindow="-16574" yWindow="3355" windowWidth="25798" windowHeight="13042" firstSheet="1" activeTab="1" xr2:uid="{42CE140A-3AB5-438F-8412-76FAA93178C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Column heads and explanation" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="168">
   <si>
     <t>KUALA LUMPUR</t>
   </si>
@@ -1267,170 +1267,286 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95004567-48F0-4B62-B4B9-4DDAF7BCD019}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="G4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>13</v>
+      <c r="A20" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>15</v>
+      <c r="A21" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>87</v>
+      <c r="A22" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>8</v>
+      <c r="A23" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1444,7 +1560,7 @@
   <dimension ref="A1:AC15"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2428,7 +2544,7 @@
         <v>131</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F13" si="0">_xlfn.CONCAT(B3, "@", E3)</f>
+        <f t="shared" ref="F3:F12" si="0">_xlfn.CONCAT(B3, "@", E3)</f>
         <v>ali@b.com</v>
       </c>
     </row>
@@ -2633,7 +2749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8F4F11-691E-4A24-8F82-DE8341AE0D7F}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>